<commit_message>
Criação e atualização de diretórios e arquivos.
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB3AA3D-AD34-45E5-8382-08078D816BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CFBBD3-EA3F-43AB-A68D-804C7B9CB656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Certificados, cursos, badges" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="161">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>https://github.com/Phelipe-Sempreboni/certificates/blob/main/dama-brasil/dama-meeting-2024/certificado.pdf</t>
+  </si>
+  <si>
+    <t>Databricks: trabalhando com diversos formatos e tipos de arquivos</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/0c532a4c-90c6-44e9-850e-b99ee7137f0d</t>
   </si>
 </sst>
 </file>
@@ -912,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2700,6 +2706,32 @@
       </c>
       <c r="I69" s="3">
         <v>45469</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D70" s="2">
+        <v>8</v>
+      </c>
+      <c r="E70" s="3">
+        <v>45479</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" s="3">
+        <v>45479</v>
       </c>
     </row>
   </sheetData>
@@ -2774,9 +2806,10 @@
     <hyperlink ref="F67" r:id="rId64" xr:uid="{341D9379-7D22-4312-B0F3-1AE58A2C88EA}"/>
     <hyperlink ref="F68" r:id="rId65" xr:uid="{10CC71D6-CF99-4C08-A3D2-85ADF1B347D1}"/>
     <hyperlink ref="F69" r:id="rId66" xr:uid="{EE66BBB2-5C47-4DAD-A91F-F3107993F671}"/>
+    <hyperlink ref="F70" r:id="rId67" xr:uid="{E23230FF-DF9A-47AF-8550-586A3D870267}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId67"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -2784,8 +2817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2E6427-F1D9-4BBB-9AE6-87A9017765C2}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Criação e atualização de diretório e arquivo.
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8AC482-EC54-4849-9DA4-8AD07E3860E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C84E9E6-5677-4B6C-BC70-D8F9BFE036A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="176">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>Databricks para líderes empresariais</t>
+  </si>
+  <si>
+    <t>https://github.com/Phelipe-Sempreboni/certificates/blob/main/databricks-academy/fundamentals/databricks-l%C3%ADderes-empresariais/certificado.pdf</t>
+  </si>
+  <si>
+    <t>Acreditação Fundamentais Databricks - Português BR</t>
   </si>
 </sst>
 </file>
@@ -959,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2928,7 +2934,9 @@
       <c r="E77" s="3">
         <v>45580</v>
       </c>
-      <c r="F77" s="4"/>
+      <c r="F77" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="G77" s="2" t="s">
         <v>28</v>
       </c>
@@ -2940,14 +2948,28 @@
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="3"/>
+      <c r="B78" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="3">
+        <v>45584</v>
+      </c>
       <c r="F78" s="4"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="3"/>
+      <c r="G78" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I78" s="3">
+        <v>45584</v>
+      </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
@@ -3087,9 +3109,10 @@
     <hyperlink ref="F73" r:id="rId70" xr:uid="{9C82B1C1-23C2-48F3-8EC8-BE2C01C25B5F}"/>
     <hyperlink ref="F74" r:id="rId71" xr:uid="{382CA266-F562-4F76-B5B9-7A80EFE9AEF0}"/>
     <hyperlink ref="F75" r:id="rId72" xr:uid="{6FC7A8BD-0CC4-4D30-82DA-CE7464C3A6B6}"/>
+    <hyperlink ref="F77" r:id="rId73" xr:uid="{285430CB-637C-4BC8-9FF4-7736E81B6C60}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId73"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Criação de diretórios e atualização de arquivos
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BE8086-202C-4490-92AB-9E95A8CFB72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B50CDAC-3845-4344-8F7B-FACC9756B811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Certificados, cursos, badges" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="221">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -697,10 +697,13 @@
     <t>DuckDB e Firecrawl Para Database e Web Scraping Analytics (Artificial Intelligence and AI Agents)</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://mycourse.app/mxMUAQev361wYF7F0</t>
-  </si>
-  <si>
     <t xml:space="preserve"> IA Generativa e Agentes de IA Para Fluxos de Automação com Langflow e n8n</t>
+  </si>
+  <si>
+    <t>https://mycourse.app/VDzetUOyz0DjHrSCP</t>
+  </si>
+  <si>
+    <t>https://mycourse.app/mxMUAQev361wYF7F0</t>
   </si>
 </sst>
 </file>
@@ -775,15 +778,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1101,27 +1101,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C82" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1" hidden="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>27</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>27</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>44744</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>65</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>27</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>27</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>113</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>113</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>45104</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>65</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>27</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>45151</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>65</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>102</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>45227</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>113</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>113</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>27</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>45388</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>27</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>45388</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>66</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>45389</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>66</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>27</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>45396</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>27</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>45396</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>27</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>27</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>27</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>27</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>27</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>27</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>27</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>45435</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>27</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
         <v>27</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>144</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>45441</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>157</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>45469</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>27</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>45479</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
         <v>27</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>45494</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>27</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>65</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>45534</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>65</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>65</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>171</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>172</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>45580</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>172</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>45584</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>172</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>45584</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>181</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
         <v>27</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>45622</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
         <v>27</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>45626</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
         <v>188</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>45645</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="2" t="s">
         <v>188</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>45645</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="2" t="s">
         <v>66</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>45298</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="2" t="s">
         <v>66</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>45690</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="2" t="s">
         <v>66</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>45690</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="2" t="s">
         <v>66</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>45690</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="2" t="s">
         <v>27</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>45692</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="2" t="s">
         <v>188</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>45692</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="2" t="s">
         <v>66</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>45711</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="2" t="s">
         <v>66</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>45711</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="2" t="s">
         <v>66</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>45711</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="2" t="s">
         <v>188</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
         <v>65</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>45789</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="2" t="s">
         <v>65</v>
       </c>
@@ -3591,12 +3591,12 @@
         <v>45846</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D97" s="2">
         <v>8</v>
@@ -3605,7 +3605,7 @@
         <v>45848</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>28</v>
@@ -3617,8 +3617,31 @@
         <v>45848</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="5"/>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B98" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D98" s="2">
+        <v>8</v>
+      </c>
+      <c r="E98" s="3">
+        <v>45849</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I98" s="3">
+        <v>45849</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:I68" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}"/>
@@ -3719,9 +3742,11 @@
     <hyperlink ref="F94" r:id="rId91" location="acc.qoPhQyrb" xr:uid="{C0AA55BB-BB9C-4067-81F7-112117003AFC}"/>
     <hyperlink ref="F95" r:id="rId92" xr:uid="{27EE5898-894D-4987-A2C5-1690C49BDB65}"/>
     <hyperlink ref="F96" r:id="rId93" xr:uid="{80A89DB6-BCAC-435B-9C81-EED713C56E41}"/>
+    <hyperlink ref="F98" r:id="rId94" xr:uid="{4CD41B68-522B-420B-80E8-260CEDC1D5D1}"/>
+    <hyperlink ref="F97" r:id="rId95" xr:uid="{9AEA2F87-2CC5-480F-BCE7-F9B2A16EA451}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId94"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId96"/>
 </worksheet>
 </file>
 
@@ -3733,23 +3758,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1" hidden="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>154</v>
       </c>
@@ -3775,7 +3800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>150</v>
       </c>
@@ -3801,7 +3826,7 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>152</v>
       </c>
@@ -3827,7 +3852,7 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>151</v>
       </c>
@@ -3853,7 +3878,7 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Criação e atualização de arquivo
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A64ACD2-CD4C-4FD1-9874-D3C20D091564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235569CA-3EF5-44C9-922B-B34A44D3711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="226">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -710,13 +710,22 @@
   </si>
   <si>
     <t>https://ude.my/UC-3fe7c102-7144-4f7d-8b4b-8db9e3407556</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/credentials/share/pt-br/PhelipeSempreboni-3357/929BE7AE09C2BBAF?sharingId=3E1FB82E24C4C34E</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>AZ-900 - Microsoft Certified: Conceitos básicos do Azure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,6 +752,14 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -790,7 +807,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1106,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3650,7 +3667,7 @@
         <v>45849</v>
       </c>
     </row>
-    <row r="99" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="2" t="s">
         <v>66</v>
       </c>
@@ -3663,7 +3680,7 @@
       <c r="E99" s="3">
         <v>45883</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="4" t="s">
         <v>222</v>
       </c>
       <c r="G99" s="2" t="s">
@@ -3675,6 +3692,44 @@
       <c r="I99" s="3">
         <v>45883</v>
       </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B100" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
+      <c r="E100" s="3">
+        <v>45891</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I100" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C106" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E109" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:I68" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}"/>
@@ -3778,9 +3833,10 @@
     <hyperlink ref="F98" r:id="rId94" xr:uid="{4CD41B68-522B-420B-80E8-260CEDC1D5D1}"/>
     <hyperlink ref="F97" r:id="rId95" xr:uid="{9AEA2F87-2CC5-480F-BCE7-F9B2A16EA451}"/>
     <hyperlink ref="F99" r:id="rId96" xr:uid="{BF7FE888-6AC5-4CF1-A7D7-6C88F5288AF2}"/>
+    <hyperlink ref="F100" r:id="rId97" xr:uid="{556F71FB-389E-4625-B8BB-9572ED4ACE68}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId97"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId98"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Criação de diretórios, arquivos e atualizações
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235569CA-3EF5-44C9-922B-B34A44D3711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EE9E86-672B-4DB8-B2BF-69F8A16BF353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="228">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>AZ-900 - Microsoft Certified: Conceitos básicos do Azure</t>
+  </si>
+  <si>
+    <t>DP-900 Azure Data Fundamentals Exam - Prep In One Day</t>
+  </si>
+  <si>
+    <t>ude.my/UC-4d2736be-92da-425f-a676-546cd07aaf8a</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1132,7 @@
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3720,7 +3726,30 @@
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B101" s="5"/>
+      <c r="B101" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D101" s="2">
+        <v>5</v>
+      </c>
+      <c r="E101" s="3">
+        <v>45902</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101" s="3">
+        <v>45902</v>
+      </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="5"/>

</xml_diff>

<commit_message>
Atualização e criação de diretórios e arquivos
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\certificates\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7A4C43-0BBA-4CEB-93A0-C30998697B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B25E83-EB4A-4C04-BAF8-9875E5E2586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="254">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>Ciências da Computação</t>
+  </si>
+  <si>
+    <t>Formação Engenheiro de Dados 4</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B85" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4126,6 +4129,30 @@
         <v>28</v>
       </c>
       <c r="I113" s="3">
+        <v>46024</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
+      </c>
+      <c r="E114" s="3">
+        <v>46024</v>
+      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I114" s="3">
         <v>46024</v>
       </c>
     </row>
@@ -4256,7 +4283,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>